<commit_message>
write methods to excel api
</commit_message>
<xml_diff>
--- a/src/com/nglcode/files/TestData.xlsx
+++ b/src/com/nglcode/files/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -34,12 +34,18 @@
     <t xml:space="preserve">NoOfAttempts</t>
   </si>
   <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
     <t xml:space="preserve">AdminUser</t>
   </si>
   <si>
     <t xml:space="preserve">admin@123</t>
   </si>
   <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">BaseUser</t>
   </si>
   <si>
@@ -56,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">super@123</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -188,11 +203,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -210,6 +229,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,88 +261,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.49"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="14.67" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.0" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="17.84" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="20.5" collapsed="false" outlineLevel="0"/>
+    <col min="16384" max="16384" customWidth="true" hidden="false" style="1" width="10.49" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="n">
         <v>42736</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>10</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="n">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9" t="n">
         <v>42795</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="8" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7" t="n">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="n">
         <v>42856</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="8" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="n">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="n">
         <v>42917</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="8" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>